<commit_message>
Added one hot encoding
</commit_message>
<xml_diff>
--- a/CE_longitudinal_codebook.xlsx
+++ b/CE_longitudinal_codebook.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I69"/>
+  <dimension ref="A1:I82"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,7 +421,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="23" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
     <col width="60" customWidth="1" min="4" max="4"/>
@@ -972,7 +972,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>['THE', 'CMS', 'OTHER:GERMAN_STUDIES', 'EDU', 'ANT', 'PSY', 'ENV', 'ART']</t>
+          <t>['THE', 'CMS', 'GRS', 'EDU', 'ANT', 'PSY', 'ENV', 'ART']</t>
         </is>
       </c>
     </row>
@@ -3424,6 +3424,487 @@
       <c r="I69" t="inlineStr">
         <is>
           <t>[1, 2, 3, 4, 5]</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Media_repost_events</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G70" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Media CE: Reposting information about current events</t>
+        </is>
+      </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Media_sign_petition</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G71" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>Media CE: Signing online petitions</t>
+        </is>
+      </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Media_follow_news</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr"/>
+      <c r="D72" t="inlineStr"/>
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G72" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>Media CE: Following accounts/pages about current events</t>
+        </is>
+      </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>[1, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Media_follow_officials</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G73" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>Media CE: Following elected officials on social media</t>
+        </is>
+      </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Media_debate_opinions</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G74" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>Media CE: Debating opinions with others who disagree</t>
+        </is>
+      </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Media_like_posts</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr"/>
+      <c r="D75" t="inlineStr"/>
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G75" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>Media CE: Liking posts about current events</t>
+        </is>
+      </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Media_post_opinions</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr"/>
+      <c r="D76" t="inlineStr"/>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G76" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>Media CE: Posting own opinions about current events</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>News_The_Elm</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G77" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>Local news: The Elm</t>
+        </is>
+      </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>[1, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>News_Kent_County</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G78" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>Local news: Kent County News</t>
+        </is>
+      </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>News_Chestertown_Spy</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr"/>
+      <c r="D79" t="inlineStr"/>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G79" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>Local news: The Chestertown Spy</t>
+        </is>
+      </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>News_Eastern_Shore_Post</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr"/>
+      <c r="D80" t="inlineStr"/>
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G80" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>Local news: Eastern Shore Post</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>News_Shore_Daily</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr"/>
+      <c r="D81" t="inlineStr"/>
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G81" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>Local news: Shore Daily News</t>
+        </is>
+      </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>News_Delmarva_Now</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G82" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>Local news: Delmarva Now</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Final coding updates for the night
</commit_message>
<xml_diff>
--- a/CE_longitudinal_codebook.xlsx
+++ b/CE_longitudinal_codebook.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I82"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,7 +421,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="26" customWidth="1" min="1" max="1"/>
     <col width="21" customWidth="1" min="2" max="2"/>
     <col width="60" customWidth="1" min="3" max="3"/>
     <col width="60" customWidth="1" min="4" max="4"/>
@@ -1938,7 +1938,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>[2, 'The Chestertown or local community', 5, 'Somewhere else (please specify)']</t>
+          <t>[2, 1, 5, 4]</t>
         </is>
       </c>
     </row>
@@ -3430,7 +3430,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Media_repost_events</t>
+          <t>CEdef_voting</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -3455,19 +3455,19 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>Media CE: Reposting information about current events</t>
+          <t>CE definition: Voting</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>[0, 1]</t>
+          <t>[1, 0]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Media_sign_petition</t>
+          <t>CEdef_volunteering</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -3492,7 +3492,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>Media CE: Signing online petitions</t>
+          <t>CE definition: Volunteering or community service</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -3504,7 +3504,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Media_follow_news</t>
+          <t>CEdef_talking_community</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -3529,19 +3529,19 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>Media CE: Following accounts/pages about current events</t>
+          <t>CE definition: Talking with people in the community</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>[1, 0]</t>
+          <t>[0, 1]</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Media_follow_officials</t>
+          <t>CEdef_activism</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3566,7 +3566,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>Media CE: Following elected officials on social media</t>
+          <t>CE definition: Activism or awareness raising</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
@@ -3578,7 +3578,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Media_debate_opinions</t>
+          <t>CEdef_political</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -3603,7 +3603,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>Media CE: Debating opinions with others who disagree</t>
+          <t>CE definition: Political engagement</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -3615,7 +3615,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Media_like_posts</t>
+          <t>CEdef_protesting</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -3640,7 +3640,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>Media CE: Liking posts about current events</t>
+          <t>CE definition: Protesting or rallying</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -3652,7 +3652,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Media_post_opinions</t>
+          <t>CEdef_teaching</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -3677,7 +3677,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>Media CE: Posting own opinions about current events</t>
+          <t>CE definition: Teaching or mentorship</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -3689,7 +3689,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>News_The_Elm</t>
+          <t>CEdef_fundraising</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3714,19 +3714,19 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>Local news: The Elm</t>
+          <t>CE definition: Fundraising</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>[1, 0]</t>
+          <t>[0, 1]</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>News_Kent_County</t>
+          <t>CEdef_arts_culture</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3751,7 +3751,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>Local news: Kent County News</t>
+          <t>CE definition: Attending community arts and culture events</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -3763,7 +3763,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>News_Chestertown_Spy</t>
+          <t>CEdef_community_business</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -3788,7 +3788,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>Local news: The Chestertown Spy</t>
+          <t>CE definition: Contributing to community businesses with a social cause</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -3800,7 +3800,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>News_Eastern_Shore_Post</t>
+          <t>CEdef_donations</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -3825,7 +3825,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>Local news: Eastern Shore Post</t>
+          <t>CE definition: Making donations to charities</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -3837,7 +3837,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>News_Shore_Daily</t>
+          <t>CEdef_research</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -3862,7 +3862,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>Local news: Shore Daily News</t>
+          <t>CE definition: Participating in research with community members</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
@@ -3874,7 +3874,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>News_Delmarva_Now</t>
+          <t>CEdef_service_learning</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -3899,10 +3899,491 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
+          <t>CE definition: Service-learning experiences with a class</t>
+        </is>
+      </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Media_repost_events</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G83" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>Media CE: Reposting information about current events</t>
+        </is>
+      </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Media_sign_petition</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr"/>
+      <c r="D84" t="inlineStr"/>
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G84" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>Media CE: Signing online petitions</t>
+        </is>
+      </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Media_follow_news</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr"/>
+      <c r="D85" t="inlineStr"/>
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G85" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>Media CE: Following accounts/pages about current events</t>
+        </is>
+      </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>[1, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Media_follow_officials</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr"/>
+      <c r="D86" t="inlineStr"/>
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G86" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>Media CE: Following elected officials on social media</t>
+        </is>
+      </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Media_debate_opinions</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr"/>
+      <c r="D87" t="inlineStr"/>
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G87" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Media CE: Debating opinions with others who disagree</t>
+        </is>
+      </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Media_like_posts</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr"/>
+      <c r="D88" t="inlineStr"/>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G88" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>Media CE: Liking posts about current events</t>
+        </is>
+      </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Media_post_opinions</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr"/>
+      <c r="D89" t="inlineStr"/>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G89" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>Media CE: Posting own opinions about current events</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>News_The_Elm</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G90" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>Local news: The Elm</t>
+        </is>
+      </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>[1, 0]</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>News_Kent_County</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G91" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>Local news: Kent County News</t>
+        </is>
+      </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>News_Chestertown_Spy</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr"/>
+      <c r="D92" t="inlineStr"/>
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G92" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>Local news: The Chestertown Spy</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>News_Eastern_Shore_Post</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr"/>
+      <c r="D93" t="inlineStr"/>
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G93" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>Local news: Eastern Shore Post</t>
+        </is>
+      </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>News_Shore_Daily</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr"/>
+      <c r="D94" t="inlineStr"/>
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G94" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Local news: Shore Daily News</t>
+        </is>
+      </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>[0, 1]</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>News_Delmarva_Now</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr"/>
+      <c r="D95" t="inlineStr"/>
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>binary OHE</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>1=selected, 0=not selected, -9=missing</t>
+        </is>
+      </c>
+      <c r="G95" t="n">
+        <v>-9</v>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
           <t>Local news: Delmarva Now</t>
         </is>
       </c>
-      <c r="I82" t="inlineStr">
+      <c r="I95" t="inlineStr">
         <is>
           <t>[0, 1]</t>
         </is>

</xml_diff>

<commit_message>
merging before closing codespace
</commit_message>
<xml_diff>
--- a/CE_longitudinal_codebook.xlsx
+++ b/CE_longitudinal_codebook.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -979,32 +979,32 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Minor_raw</t>
+          <t>Transfer_student</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>QID45_TEXT</t>
+          <t>QID46</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>SP23:— / SP24:Q45 / SP25:Q45</t>
+          <t>SP23:— / SP24:Q46 / SP25:Q46</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>What is your minor or intended minor? (Double or triple minors, please list all below)</t>
+          <t>Are you a transfer student?</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Open response; -9 for SP23 (not asked)</t>
+          <t>1=Yes, 0=No; -9 for SP23</t>
         </is>
       </c>
       <c r="G15" t="n">
@@ -1012,28 +1012,36 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Raw minor text; only asked SP24/SP25</t>
+          <t>Transfer student? (asked SP24/SP25 only)</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>['Elementary Ed Cert ', 'Elementary Education Certification ', 'Museum, Field, and Community Education', 'Education ', '</t>
+          <t>[0, 1]</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Minor1</t>
+          <t>Gender</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
+          <t>QID28</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>SP23:Q23 / SP24:Q23 / SP25:Q23</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>What best describes your gender identity?</t>
+        </is>
+      </c>
       <c r="E16" t="inlineStr">
         <is>
           <t>categorical</t>
@@ -1041,7 +1049,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>WC 3-letter catalog code or ''</t>
+          <t>1=Man, 2=Woman, 3=Non-binary, 4=Self-describe, 5=Prefer not</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1049,36 +1057,44 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Minor recoded from Minor_raw or 'with minor' in Major_raw</t>
+          <t>Gender identity</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>['OTHER:ELEMENTARY_ED_CERT', 'UNDECLARED', 'EDU', 'OTHER:MUSEUM; OTHER:FIELD; EDU', 'MFCE; ANT', 'CHE', 'DAN', 'OTHER:MA</t>
+          <t>[2, 1, 6, 3, 5, 4]</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Major_minor_inferred</t>
+          <t>Race_ethnicity</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
+          <t>QID29</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>SP23:Q24 / SP24:Q24 / SP25:Q24</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>What is your racial and/or ethnic identity? Select all that apply.</t>
+        </is>
+      </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>categorical</t>
+          <t>multi-select text</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>WC code or ''</t>
+          <t>Open response / multi-select</t>
         </is>
       </c>
       <c r="G17" t="n">
@@ -1086,44 +1102,44 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Minor inferred from phrasing in Major_raw field</t>
+          <t>Racial/ethnic identity</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['European American or White', 'European American or White,Hispanic/Latinx', 'Indigenous/Hawaiian/Pacific Islander', 'Af</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Transfer_student</t>
+          <t>Participant_code</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>QID46</t>
+          <t>QID44_TEXT</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>SP23:— / SP24:Q46 / SP25:Q46</t>
+          <t>SP23:Q44 / SP24:Q44 / SP25:Q44</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Are you a transfer student?</t>
+          <t>If you are taking this survey for course credit, please add your participant number here.</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>binary</t>
+          <t>text</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>1=Yes, 0=No; -9 for SP23</t>
+          <t>Open response</t>
         </is>
       </c>
       <c r="G18" t="n">
@@ -1131,89 +1147,81 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Transfer student? (asked SP24/SP25 only)</t>
+          <t>Course-credit participant number</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>[0, 1]</t>
+          <t>['', '17', '55', '73', '36', '84', '14', '68']</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Gender</t>
+          <t>EndDate</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>QID28</t>
+          <t>endDate</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>SP23:Q23 / SP24:Q23 / SP25:Q23</t>
+          <t>SP23:EndDate / SP24:EndDate / SP25:EndDate</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>What best describes your gender identity?</t>
+          <t>End Date</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>categorical</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>1=Man, 2=Woman, 3=Non-binary, 4=Self-describe, 5=Prefer not</t>
-        </is>
-      </c>
+          <t>text</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="n">
         <v>-9</v>
       </c>
-      <c r="H19" t="inlineStr">
-        <is>
-          <t>Gender identity</t>
-        </is>
-      </c>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="inlineStr">
         <is>
-          <t>[2, 1, 6, 3, 5, 4]</t>
+          <t>['2023-03-28 11:59:12', '2023-03-28 12:37:32', '2023-03-28 12:38:29', '2023-03-28 12:39:11', '2023-03-28 12:39:12', '202</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Race_ethnicity</t>
+          <t>Consent</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>QID29</t>
+          <t>QID37</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>SP23:Q24 / SP24:Q24 / SP25:Q24</t>
+          <t>SP23:Consent / SP24:Consent / SP25:Consent</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>What is your racial and/or ethnic identity? Select all that apply.</t>
+          <t>I am a current Washington College student and I agree to participate in this survey.</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>multi-select text</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Open response / multi-select</t>
+          <t>1=Agreed, 0=Not agreed</t>
         </is>
       </c>
       <c r="G20" t="n">
@@ -1221,34 +1229,34 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Racial/ethnic identity</t>
+          <t>Qualtrics consent gate</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>['European American or White', 'European American or White,Hispanic/Latinx', 'Indigenous/Hawaiian/Pacific Islander', 'Af</t>
+          <t>['Yes (continue to survey)', 'No (end survey)']</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Participant_code</t>
+          <t>CE_definition_text</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>QID44_TEXT</t>
+          <t>QID2</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>SP23:Q44 / SP24:Q44 / SP25:Q44</t>
+          <t>SP23:Q2- Text / SP24:Q2- Text / SP25:Q2- Text</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>If you are taking this survey for course credit, please add your participant number here.</t>
+          <t>There are many definitions of civic engagement.     Civic engagement is individual and collective actions designed to identify and address issues of public concern and opportunities for positive chang</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1258,7 +1266,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Open response</t>
+          <t>Displayed text passage</t>
         </is>
       </c>
       <c r="G21" t="n">
@@ -1266,34 +1274,34 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Course-credit participant number</t>
+          <t>Civic engagement definition shown to respondent</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>['', '17', '55', '73', '36', '84', '14', '68']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>EndDate</t>
+          <t>CE_define_open</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>endDate</t>
+          <t>QID3</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>SP23:EndDate / SP24:EndDate / SP25:EndDate</t>
+          <t>SP23:Q3- Define CE / SP24:Q3- Define CE / SP25:Q3- Define CE</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>End Date</t>
+          <t>When you think about civic engagement, what activities are central to your definition, or are most important?   Check all that apply</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1301,46 +1309,54 @@
           <t>text</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Open response</t>
+        </is>
+      </c>
       <c r="G22" t="n">
         <v>-9</v>
       </c>
-      <c r="H22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Respondent's own definition of civic engagement</t>
+        </is>
+      </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>['2023-03-28 11:59:12', '2023-03-28 12:37:32', '2023-03-28 12:38:29', '2023-03-28 12:39:11', '2023-03-28 12:39:12', '202</t>
+          <t>['Voting', 'Voting,Political engagement,Talking with people in the community,Fundraising,Volunteering or doing community</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Consent</t>
+          <t>CESA_1</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>QID37</t>
+          <t>QID4_1</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>SP23:Consent / SP24:Consent / SP25:Consent</t>
+          <t>SP23:Q4-CESA_1 / SP24:Q4-CESA_1 / SP25:Q4-CESA_1</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>I am a current Washington College student and I agree to participate in this survey.</t>
+          <t>Questions about Civic Engagement Attitudes     Civic engagement attitudes are your personal beliefs and feelings about your own involvement in your community and your ability to make a difference ther</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>binary</t>
+          <t>Likert-5</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>1=Agreed, 0=Not agreed</t>
+          <t>1=Strongly disagree…5=Strongly agree</t>
         </is>
       </c>
       <c r="G23" t="n">
@@ -1348,44 +1364,44 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Qualtrics consent gate</t>
+          <t>CESA item 1</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>['Yes (continue to survey)', 'No (end survey)']</t>
+          <t>[2, 4, 3]</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CE_definition_text</t>
+          <t>CESA_2</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>QID2</t>
+          <t>QID4_5</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>SP23:Q2- Text / SP24:Q2- Text / SP25:Q2- Text</t>
+          <t>SP23:Q4-CESA_2 / SP24:Q4-CESA_2 / SP25:Q4-CESA_2</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>There are many definitions of civic engagement.     Civic engagement is individual and collective actions designed to identify and address issues of public concern and opportunities for positive chang</t>
+          <t>Questions about Civic Engagement Attitudes     Civic engagement attitudes are your personal beliefs and feelings about your own involvement in your community and your ability to make a difference ther</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>Likert-5</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Displayed text passage</t>
+          <t>1=Strongly disagree…5=Strongly agree</t>
         </is>
       </c>
       <c r="G24" t="n">
@@ -1393,44 +1409,44 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Civic engagement definition shown to respondent</t>
+          <t>CESA item 2</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[2, 4, 3]</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CE_define_open</t>
+          <t>CESA_3</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>QID3</t>
+          <t>QID4_3</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>SP23:Q3- Define CE / SP24:Q3- Define CE / SP25:Q3- Define CE</t>
+          <t>SP23:Q4-CESA_3 / SP24:Q4-CESA_3 / SP25:Q4-CESA_3</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>When you think about civic engagement, what activities are central to your definition, or are most important?   Check all that apply</t>
+          <t>Questions about Civic Engagement Attitudes     Civic engagement attitudes are your personal beliefs and feelings about your own involvement in your community and your ability to make a difference ther</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>Likert-5</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Open response</t>
+          <t>1=Strongly disagree…5=Strongly agree</t>
         </is>
       </c>
       <c r="G25" t="n">
@@ -1438,29 +1454,29 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>Respondent's own definition of civic engagement</t>
+          <t>CESA item 3</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>['Voting', 'Voting,Political engagement,Talking with people in the community,Fundraising,Volunteering or doing community</t>
+          <t>[2, 4, 3]</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CESA_1</t>
+          <t>CESA_4</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>QID4_1</t>
+          <t>QID4_4</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>SP23:Q4-CESA_1 / SP24:Q4-CESA_1 / SP25:Q4-CESA_1</t>
+          <t>SP23:Q4-CESA_4 / SP24:Q4-CESA_4 / SP25:Q4-CESA_4</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1483,7 +1499,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>CESA item 1</t>
+          <t>CESA item 4</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
@@ -1495,17 +1511,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CESA_2</t>
+          <t>CESA_5</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>QID4_5</t>
+          <t>QID4_11</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>SP23:Q4-CESA_2 / SP24:Q4-CESA_2 / SP25:Q4-CESA_2</t>
+          <t>SP23:Q4-CESA_5 / SP24:Q4-CESA_5 / SP25:Q4-CESA_5</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1528,29 +1544,29 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>CESA item 2</t>
+          <t>CESA item 5</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>[2, 4, 3]</t>
+          <t>[2, 3, 4]</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CESA_3</t>
+          <t>CESA_6</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>QID4_3</t>
+          <t>QID4_12</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>SP23:Q4-CESA_3 / SP24:Q4-CESA_3 / SP25:Q4-CESA_3</t>
+          <t>SP23:Q4-CESA_6 / SP24:Q4-CESA_6 / SP25:Q4-CESA_6</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1573,29 +1589,29 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>CESA item 3</t>
+          <t>CESA item 6</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>[2, 4, 3]</t>
+          <t>[2, 3, 4]</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CESA_4</t>
+          <t>CESA_7</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>QID4_4</t>
+          <t>QID4_6</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>SP23:Q4-CESA_4 / SP24:Q4-CESA_4 / SP25:Q4-CESA_4</t>
+          <t>SP23:Q4-CESA_7 / SP24:Q4-CESA_7 / SP25:Q4-CESA_7</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1618,7 +1634,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>CESA item 4</t>
+          <t>CESA item 7</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -1630,17 +1646,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CESA_5</t>
+          <t>CESA_8</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>QID4_11</t>
+          <t>QID4_7</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SP23:Q4-CESA_5 / SP24:Q4-CESA_5 / SP25:Q4-CESA_5</t>
+          <t>SP23:Q4-CESA_8 / SP24:Q4-CESA_8 / SP25:Q4-CESA_8</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1663,29 +1679,29 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>CESA item 5</t>
+          <t>CESA item 8</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>[2, 3, 4]</t>
+          <t>[2, 4, 3]</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CESA_6</t>
+          <t>CESA_9</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>QID4_12</t>
+          <t>QID4_8</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>SP23:Q4-CESA_6 / SP24:Q4-CESA_6 / SP25:Q4-CESA_6</t>
+          <t>SP23:Q4-CESA_9 / SP24:Q4-CESA_9 / SP25:Q4-CESA_9</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1708,29 +1724,29 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>CESA item 6</t>
+          <t>CESA item 9</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>[2, 3, 4]</t>
+          <t>[2, 4, 3]</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CESA_7</t>
+          <t>CESA_10</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>QID4_6</t>
+          <t>QID4_9</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>SP23:Q4-CESA_7 / SP24:Q4-CESA_7 / SP25:Q4-CESA_7</t>
+          <t>SP23:Q4-CESA_10 / SP24:Q4-CESA_10 / SP25:Q4-CESA_10</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
@@ -1753,7 +1769,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>CESA item 7</t>
+          <t>CESA item 10</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -1765,32 +1781,32 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CESA_8</t>
+          <t>Community_ref</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>QID4_7</t>
+          <t>QID6</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>SP23:Q4-CESA_8 / SP24:Q4-CESA_8 / SP25:Q4-CESA_8</t>
+          <t>SP23:Q6 / SP24:Q6 / SP25:Q6</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Questions about Civic Engagement Attitudes     Civic engagement attitudes are your personal beliefs and feelings about your own involvement in your community and your ability to make a difference ther</t>
+          <t>When answering the previous questions about community engagement, were you mostly thinking about: - Selected Choice</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Likert-5</t>
+          <t>categorical</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>1=Strongly disagree…5=Strongly agree</t>
+          <t>1=Chestertown, 2=WC, 3=National, 4=Other, 5=Home</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -1798,44 +1814,44 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>CESA item 8</t>
+          <t>Which community respondent referenced for prior Qs</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>[2, 4, 3]</t>
+          <t>[2, 1, 5, 4]</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CESA_9</t>
+          <t>Community_ref_other</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>QID4_8</t>
+          <t>QID6_4_TEXT</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>SP23:Q4-CESA_9 / SP24:Q4-CESA_9 / SP25:Q4-CESA_9</t>
+          <t>SP23:Q6_4_TEXT / SP24:Q6_4_TEXT / SP25:Q6_4_TEXT</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Questions about Civic Engagement Attitudes     Civic engagement attitudes are your personal beliefs and feelings about your own involvement in your community and your ability to make a difference ther</t>
+          <t>When answering the previous questions about community engagement, were you mostly thinking about: - Somewhere else (please specify) - Text</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Likert-5</t>
+          <t>text</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>1=Strongly disagree…5=Strongly agree</t>
+          <t>Open response</t>
         </is>
       </c>
       <c r="G34" t="n">
@@ -1843,44 +1859,44 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>CESA item 9</t>
+          <t>Specified 'other' community</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>[2, 4, 3]</t>
+          <t xml:space="preserve">['Both a and C', 'The WAC and Chestertown communities', 'The various communities I have lived in.', 'Combination of WAC </t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CESA_10</t>
+          <t>Volunteer_yn</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>QID4_9</t>
+          <t>QID7</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>SP23:Q4-CESA_10 / SP24:Q4-CESA_10 / SP25:Q4-CESA_10</t>
+          <t>SP23:Q7-ESP1 / SP24:Q7-ESP1 / SP25:Q7-ESP1</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Questions about Civic Engagement Attitudes     Civic engagement attitudes are your personal beliefs and feelings about your own involvement in your community and your ability to make a difference ther</t>
+          <t>Engagement With Our Local Community    Many people say that they have less time these days to do volunteer work. What about you? In the past year, were you able to devote any time to volunteer work in</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Likert-5</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>1=Strongly disagree…5=Strongly agree</t>
+          <t>1=Yes, 0=No</t>
         </is>
       </c>
       <c r="G35" t="n">
@@ -1888,44 +1904,44 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>CESA item 10</t>
+          <t>Volunteer in community?</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>[2, 4, 3]</t>
+          <t>[1, 0]</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Community_ref</t>
+          <t>Volunteer_hrs_month</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>QID6</t>
+          <t>QID8</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>SP23:Q6 / SP24:Q6 / SP25:Q6</t>
+          <t>SP23:Q7a-ESP1 / SP24:Q7a-ESP1 / SP25:Q7a-ESP1</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>When answering the previous questions about community engagement, were you mostly thinking about: - Selected Choice</t>
+          <t>On average, approximately how many hours per month would you say you spend on volunteer work?</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>categorical</t>
+          <t>ordinal</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>1=Chestertown, 2=WC, 3=National, 4=Other, 5=Home</t>
+          <t>1=&lt;4 hrs, 2=4-8 hrs, 3=8-12 hrs, 4=&gt;12 hrs</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -1933,44 +1949,44 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>Which community respondent referenced for prior Qs</t>
+          <t>Avg volunteer hrs/month (ordinal bands)</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>[2, 1, 5, 4]</t>
+          <t>['8 to 12 hours per month', 'Less than 4 hours per month', '4 to 8 hours per month', 'More than 12 hours per month']</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Community_ref_other</t>
+          <t>Civic_duty_1</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>QID6_4_TEXT</t>
+          <t>QID9_1</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>SP23:Q6_4_TEXT / SP24:Q6_4_TEXT / SP25:Q6_4_TEXT</t>
+          <t>SP23:Q8-ESP2_1 / SP24:Q8-ESP2_1 / SP25:Q8-ESP2_1</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>When answering the previous questions about community engagement, were you mostly thinking about: - Somewhere else (please specify) - Text</t>
+          <t>Many people believe that everyone must do their part to help maintain a healthy community and democracy.   Regardless of how often you are personally able to engage in the following activities, please</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>text</t>
+          <t>Likert-5</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Open response</t>
+          <t>1=SD…5=SA</t>
         </is>
       </c>
       <c r="G37" t="n">
@@ -1978,44 +1994,44 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>Specified 'other' community</t>
+          <t>Civic duty scale item 1</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t xml:space="preserve">['Both a and C', 'The WAC and Chestertown communities', 'The various communities I have lived in.', 'Combination of WAC </t>
+          <t>[4, 1, 3, 2]</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Volunteer_yn</t>
+          <t>Civic_duty_2</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>QID7</t>
+          <t>QID9_2</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>SP23:Q7-ESP1 / SP24:Q7-ESP1 / SP25:Q7-ESP1</t>
+          <t>SP23:Q8-ESP2_2 / SP24:Q8-ESP2_2 / SP25:Q8-ESP2_2</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Engagement With Our Local Community    Many people say that they have less time these days to do volunteer work. What about you? In the past year, were you able to devote any time to volunteer work in</t>
+          <t>Many people believe that everyone must do their part to help maintain a healthy community and democracy.   Regardless of how often you are personally able to engage in the following activities, please</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>binary</t>
+          <t>Likert-5</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>1=Yes, 0=No</t>
+          <t>1=SD…5=SA</t>
         </is>
       </c>
       <c r="G38" t="n">
@@ -2023,44 +2039,44 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>Volunteer in community?</t>
+          <t>Civic duty scale item 2</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>[1, 0]</t>
+          <t>[4, 3, 2, 1]</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Volunteer_hrs_month</t>
+          <t>Civic_duty_3</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>QID8</t>
+          <t>QID9_3</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>SP23:Q7a-ESP1 / SP24:Q7a-ESP1 / SP25:Q7a-ESP1</t>
+          <t>SP23:Q8-ESP2_3 / SP24:Q8-ESP2_3 / SP25:Q8-ESP2_3</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>On average, approximately how many hours per month would you say you spend on volunteer work?</t>
+          <t>Many people believe that everyone must do their part to help maintain a healthy community and democracy.   Regardless of how often you are personally able to engage in the following activities, please</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>numeric</t>
+          <t>Likert-5</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Hours per month (open)</t>
+          <t>1=SD…5=SA</t>
         </is>
       </c>
       <c r="G39" t="n">
@@ -2068,29 +2084,29 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>Avg volunteer hrs/month</t>
+          <t>Civic duty scale item 3</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>['8 to 12 hours per month', 'Less than 4 hours per month', '4 to 8 hours per month', 'More than 12 hours per month']</t>
+          <t>[4, 2, 3, 1]</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Civic_duty_1</t>
+          <t>Civic_duty_4</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>QID9_1</t>
+          <t>QID9_4</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>SP23:Q8-ESP2_1 / SP24:Q8-ESP2_1 / SP25:Q8-ESP2_1</t>
+          <t>SP23:Q8-ESP2_4 / SP24:Q8-ESP2_4 / SP25:Q8-ESP2_4</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -2113,29 +2129,29 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>Civic duty scale item 1</t>
+          <t>Civic duty scale item 4</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>[4, 1, 3, 2]</t>
+          <t>[4, 2, 3, 1]</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Civic_duty_2</t>
+          <t>Civic_duty_5</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>QID9_2</t>
+          <t>QID9_5</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>SP23:Q8-ESP2_2 / SP24:Q8-ESP2_2 / SP25:Q8-ESP2_2</t>
+          <t>SP23:Q8-ESP2_5 / SP24:Q8-ESP2_5 / SP25:Q8-ESP2_5</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -2158,29 +2174,29 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>Civic duty scale item 2</t>
+          <t>Civic duty scale item 5</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>[4, 3, 2, 1]</t>
+          <t>[4, 3, 1, 2]</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Civic_duty_3</t>
+          <t>Civic_duty_6</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>QID9_3</t>
+          <t>QID9_6</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>SP23:Q8-ESP2_3 / SP24:Q8-ESP2_3 / SP25:Q8-ESP2_3</t>
+          <t>SP23:Q8-ESP2_6 / SP24:Q8-ESP2_6 / SP25:Q8-ESP2_6</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2203,44 +2219,44 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>Civic duty scale item 3</t>
+          <t>Civic duty scale item 6</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>[4, 2, 3, 1]</t>
+          <t>[4, 3, 2, 1]</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Civic_duty_4</t>
+          <t>CE_activity_1</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>QID9_4</t>
+          <t>QID31_1</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>SP23:Q8-ESP2_4 / SP24:Q8-ESP2_4 / SP25:Q8-ESP2_4</t>
+          <t>SP23:Q31_1 / SP24:Q31_1 / SP25:Q31_1</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Many people believe that everyone must do their part to help maintain a healthy community and democracy.   Regardless of how often you are personally able to engage in the following activities, please</t>
+          <t>In the last year, how often have you participated in the following activities? - Attended community meetings</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Likert-5</t>
+          <t>Likert-5 frequency</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>1=SD…5=SA</t>
+          <t>1=Never…5=Very often (weekly+)</t>
         </is>
       </c>
       <c r="G43" t="n">
@@ -2248,44 +2264,44 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>Civic duty scale item 4</t>
+          <t>CE activity frequency item 1</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>[4, 2, 3, 1]</t>
+          <t>[4, 1, 3]</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Civic_duty_5</t>
+          <t>CE_activity_2</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>QID9_5</t>
+          <t>QID31_2</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>SP23:Q8-ESP2_5 / SP24:Q8-ESP2_5 / SP25:Q8-ESP2_5</t>
+          <t>SP23:Q31_2 / SP24:Q31_2 / SP25:Q31_2</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Many people believe that everyone must do their part to help maintain a healthy community and democracy.   Regardless of how often you are personally able to engage in the following activities, please</t>
+          <t>In the last year, how often have you participated in the following activities? - Participated in volunteer work</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Likert-5</t>
+          <t>Likert-5 frequency</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>1=SD…5=SA</t>
+          <t>1=Never…5=Very often (weekly+)</t>
         </is>
       </c>
       <c r="G44" t="n">
@@ -2293,44 +2309,44 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>Civic duty scale item 5</t>
+          <t>CE activity frequency item 2</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>[4, 3, 1, 2]</t>
+          <t>[4, 3, 1]</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Civic_duty_6</t>
+          <t>CE_activity_3</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>QID9_6</t>
+          <t>QID31_3</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>SP23:Q8-ESP2_6 / SP24:Q8-ESP2_6 / SP25:Q8-ESP2_6</t>
+          <t>SP23:Q31_3 / SP24:Q31_3 / SP25:Q31_3</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Many people believe that everyone must do their part to help maintain a healthy community and democracy.   Regardless of how often you are personally able to engage in the following activities, please</t>
+          <t>In the last year, how often have you participated in the following activities? - Expressed political opinions to elected officials</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Likert-5</t>
+          <t>Likert-5 frequency</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>1=SD…5=SA</t>
+          <t>1=Never…5=Very often (weekly+)</t>
         </is>
       </c>
       <c r="G45" t="n">
@@ -2338,34 +2354,34 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>Civic duty scale item 6</t>
+          <t>CE activity frequency item 3</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>[4, 3, 2, 1]</t>
+          <t>[4, 1, 3]</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>CE_activity_1</t>
+          <t>CE_activity_4</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>QID31_1</t>
+          <t>QID31_4</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>SP23:Q31_1 / SP24:Q31_1 / SP25:Q31_1</t>
+          <t>SP23:Q31_4 / SP24:Q31_4 / SP25:Q31_4</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>In the last year, how often have you participated in the following activities? - Attended community meetings</t>
+          <t>In the last year, how often have you participated in the following activities? - Engaged in respectful political debates or discussions with those who hold different beleifes</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -2383,7 +2399,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>CE activity frequency item 1</t>
+          <t>CE activity frequency item 4</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
@@ -2395,22 +2411,22 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>CE_activity_2</t>
+          <t>CE_activity_5</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>QID31_2</t>
+          <t>QID31_5</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>SP23:Q31_2 / SP24:Q31_2 / SP25:Q31_2</t>
+          <t>SP23:Q31_5 / SP24:Q31_5 / SP25:Q31_5</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>In the last year, how often have you participated in the following activities? - Participated in volunteer work</t>
+          <t>In the last year, how often have you participated in the following activities? - Educated myself on political or social issues</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -2428,34 +2444,34 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>CE activity frequency item 2</t>
+          <t>CE activity frequency item 5</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>[4, 3, 1]</t>
+          <t>[4, 1, 3]</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>CE_activity_3</t>
+          <t>CE_activity_6</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>QID31_3</t>
+          <t>QID31_6</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>SP23:Q31_3 / SP24:Q31_3 / SP25:Q31_3</t>
+          <t>SP23:Q31_6 / SP24:Q31_6 / SP25:Q31_6</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>In the last year, how often have you participated in the following activities? - Expressed political opinions to elected officials</t>
+          <t>In the last year, how often have you participated in the following activities? - Fundraised for a cause I believe in</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -2473,44 +2489,44 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>CE activity frequency item 3</t>
+          <t>CE activity frequency item 6</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>[4, 1, 3]</t>
+          <t>[4, 3, 1]</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>CE_activity_4</t>
+          <t>Media_CE_activities</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>QID31_4</t>
+          <t>QID11</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>SP23:Q31_4 / SP24:Q31_4 / SP25:Q31_4</t>
+          <t>SP23:Q10-M1 / SP24:Q10-M1 / SP25:Q10-M1</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>In the last year, how often have you participated in the following activities? - Engaged in respectful political debates or discussions with those who hold different beleifes</t>
+          <t>The following questions are about civic engagement and media. Which of the following activities do you think count as online civic engagement? Check all that apply</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Likert-5 frequency</t>
+          <t>multi-select text</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>1=Never…5=Very often (weekly+)</t>
+          <t>Comma-separated selected options</t>
         </is>
       </c>
       <c r="G49" t="n">
@@ -2518,44 +2534,44 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>CE activity frequency item 4</t>
+          <t>Social media activities seen as CE (Q10-M1)</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>[4, 1, 3]</t>
+          <t xml:space="preserve">['Following accounts/pages that post about current events.', 'Signing online petitions.,Debating opinions or ideas with </t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>CE_activity_5</t>
+          <t>Local_news_yn</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>QID31_5</t>
+          <t>QID17</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>SP23:Q31_5 / SP24:Q31_5 / SP25:Q31_5</t>
+          <t>SP23:Q14-M6 / SP24:Q14-M6 / SP25:Q14-M6</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>In the last year, how often have you participated in the following activities? - Educated myself on political or social issues</t>
+          <t>Do you regularly read local newspapers or publications such as The Elm, the Chestertown Spy, or the Kent County News, either in print or online?</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Likert-5 frequency</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>1=Never…5=Very often (weekly+)</t>
+          <t>1=Yes, 0=No</t>
         </is>
       </c>
       <c r="G50" t="n">
@@ -2563,44 +2579,44 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>CE activity frequency item 5</t>
+          <t>Reads local news regularly?</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>[4, 1, 3]</t>
+          <t>[0, 1]</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>CE_activity_6</t>
+          <t>Local_news_which</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>QID31_6</t>
+          <t>QID18</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>SP23:Q31_6 / SP24:Q31_6 / SP25:Q31_6</t>
+          <t>SP23:Q14-M6a / SP24:Q14-M6a / SP25:Q14-M6a</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>In the last year, how often have you participated in the following activities? - Fundraised for a cause I believe in</t>
+          <t>Which local publications do you read regularly (at least once per month)? Check all that apply</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Likert-5 frequency</t>
+          <t>multi-select text</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>1=Never…5=Very often (weekly+)</t>
+          <t>Comma-separated publications</t>
         </is>
       </c>
       <c r="G51" t="n">
@@ -2608,44 +2624,44 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>CE activity frequency item 6</t>
+          <t>Which local publications read</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>[4, 3, 1]</t>
+          <t>['The Elm', 'The Elm,Kent County News', 'The Elm,The Chestertown Spy,Kent County News', 'The Elm,The Chestertown Spy,Ken</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Media_CE_activities</t>
+          <t>Local_news_connected</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>QID11</t>
+          <t>QID19</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>SP23:Q10-M1 / SP24:Q10-M1 / SP25:Q10-M1</t>
+          <t>SP23:Q14-M6b / SP24:Q14-M6b / SP25:Q14-M6b</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>The following questions are about civic engagement and media. Which of the following activities do you think count as online civic engagement? Check all that apply</t>
+          <t>How connected do you feel to the community as a result of reading local news?</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>multi-select text</t>
+          <t>Likert-5 connection</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Comma-separated selected options</t>
+          <t>1=Very disconnected…5=Very connected</t>
         </is>
       </c>
       <c r="G52" t="n">
@@ -2653,44 +2669,44 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>Social media activities seen as CE (Q10-M1)</t>
+          <t>Connection from reading local news</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t xml:space="preserve">['Following accounts/pages that post about current events.', 'Signing online petitions.,Debating opinions or ideas with </t>
+          <t>[3, 5, 4, 2, 1]</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Local_news_yn</t>
+          <t>Local_news_CE_yn</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>QID17</t>
+          <t>QID20</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>SP23:Q14-M6 / SP24:Q14-M6 / SP25:Q14-M6</t>
+          <t>SP23:Q15-M7 / SP24:Q15-M7 / SP25:Q15-M7</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Do you regularly read local newspapers or publications such as The Elm, the Chestertown Spy, or the Kent County News, either in print or online?</t>
+          <t>In your opinion, does reading local news publications count as a form of civic engagement?</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>binary</t>
+          <t>Likert-4</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>1=Yes, 0=No</t>
+          <t>1=Definitely not…4=Definitely yes</t>
         </is>
       </c>
       <c r="G53" t="n">
@@ -2698,44 +2714,44 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>Reads local news regularly?</t>
+          <t>Does reading local news count as CE?</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>[0, 1]</t>
+          <t>[4, 1]</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Local_news_which</t>
+          <t>CE_campus_1</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>QID18</t>
+          <t>QID21_1</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>SP23:Q14-M6a / SP24:Q14-M6a / SP25:Q14-M6a</t>
+          <t>SP23:Q16_1 / SP24:Q16_1 / SP25:Q16_1</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Which local publications do you read regularly (at least once per month)? Check all that apply</t>
+          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - It is important for me to stay informed about what is hap</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>multi-select text</t>
+          <t>Likert-5</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Comma-separated publications</t>
+          <t>1=SD…5=SA</t>
         </is>
       </c>
       <c r="G54" t="n">
@@ -2743,44 +2759,44 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>Which local publications read</t>
+          <t>CE campus experience Q16 item 1 (QID21_1)</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>['The Elm', 'The Elm,Kent County News', 'The Elm,The Chestertown Spy,Kent County News', 'The Elm,The Chestertown Spy,Ken</t>
+          <t>[5, 3, 4, 2, 1]</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Local_news_connected</t>
+          <t>CE_campus_2</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>QID19</t>
+          <t>QID21_2</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>SP23:Q14-M6b / SP24:Q14-M6b / SP25:Q14-M6b</t>
+          <t>SP23:Q16_2 / SP24:Q16_2 / SP25:Q16_2</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>How connected do you feel to the community as a result of reading local news?</t>
+          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - I feel accepted in the community outside of Washington Co</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Likert-5 connection</t>
+          <t>Likert-5</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>1=Very disconnected…5=Very connected</t>
+          <t>1=SD…5=SA</t>
         </is>
       </c>
       <c r="G55" t="n">
@@ -2788,44 +2804,44 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>Connection from reading local news</t>
+          <t>CE campus experience Q16 item 2 (QID21_2)</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>[3, 5, 4, 2, 1]</t>
+          <t>[5, 4, 3, 2, 1]</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Local_news_CE_yn</t>
+          <t>CE_campus_3</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>QID20</t>
+          <t>QID21_3</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>SP23:Q15-M7 / SP24:Q15-M7 / SP25:Q15-M7</t>
+          <t>SP23:Q16_3 / SP24:Q16_3 / SP25:Q16_3</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>In your opinion, does reading local news publications count as a form of civic engagement?</t>
+          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - The Chestertown community welcomes Washington College stu</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Likert-4</t>
+          <t>Likert-5</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>1=Definitely not…4=Definitely yes</t>
+          <t>1=SD…5=SA</t>
         </is>
       </c>
       <c r="G56" t="n">
@@ -2833,34 +2849,34 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>Does reading local news count as CE?</t>
+          <t>CE campus experience Q16 item 3 (QID21_3)</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>[4, 1]</t>
+          <t>[5, 1, 4, 3, 2]</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>CE_campus_1</t>
+          <t>CE_campus_4</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>QID21_1</t>
+          <t>QID21_4</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>SP23:Q16_1 / SP24:Q16_1 / SP25:Q16_1</t>
+          <t>SP23:Q16_4 / SP24:Q16_4 / SP25:Q16_4</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - It is important for me to stay informed about what is hap</t>
+          <t xml:space="preserve">Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - It is important for students to participate in community </t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -2878,34 +2894,34 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>CE campus experience Q16 item 1 (QID21_1)</t>
+          <t>CE campus experience Q16 item 4 (QID21_4)</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>[5, 3, 4, 2, 1]</t>
+          <t>[5, 4, 3, 2, 1]</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>CE_campus_2</t>
+          <t>CE_campus_5</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>QID21_2</t>
+          <t>QID21_5</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>SP23:Q16_2 / SP24:Q16_2 / SP25:Q16_2</t>
+          <t>SP23:Q16_5 / SP24:Q16_5 / SP25:Q16_5</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - I feel accepted in the community outside of Washington Co</t>
+          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - Washington College makes positive contributions to the su</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
@@ -2923,7 +2939,7 @@
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>CE campus experience Q16 item 2 (QID21_2)</t>
+          <t>CE campus experience Q16 item 5 (QID21_5)</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
@@ -2935,22 +2951,22 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>CE_campus_3</t>
+          <t>CE_campus_6</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>QID21_3</t>
+          <t>QID21_6</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>SP23:Q16_3 / SP24:Q16_3 / SP25:Q16_3</t>
+          <t>SP23:Q16_6 / SP24:Q16_6 / SP25:Q16_6</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - The Chestertown community welcomes Washington College stu</t>
+          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - Washington College supports student civic engagement</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2968,34 +2984,34 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>CE campus experience Q16 item 3 (QID21_3)</t>
+          <t>CE campus experience Q16 item 6 (QID21_6)</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>[5, 1, 4, 3, 2]</t>
+          <t>[5, 1, 3, 2, 4]</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>CE_campus_4</t>
+          <t>CE_campus_7</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>QID21_4</t>
+          <t>QID21_7</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>SP23:Q16_4 / SP24:Q16_4 / SP25:Q16_4</t>
+          <t>SP23:Q16_7 / SP24:Q16_8 / SP25:Q16_8</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t xml:space="preserve">Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - It is important for students to participate in community </t>
+          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - It is my responsibility to leave Washington College bette</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
@@ -3013,7 +3029,7 @@
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>CE campus experience Q16 item 4 (QID21_4)</t>
+          <t>CE campus item QID21_7: SP23=Q16_7, SP24/25=Q16_8 (renumbered due to new Q16_7 in SP24+)</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
@@ -3025,22 +3041,22 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>CE_campus_5</t>
+          <t>CE_campus_8</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>QID21_5</t>
+          <t>QID21_8</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>SP23:Q16_5 / SP24:Q16_5 / SP25:Q16_5</t>
+          <t>SP23:Q16_8 / SP24:Q16_9 / SP25:Q16_9</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - Washington College makes positive contributions to the su</t>
+          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - It is my responsibility to leave Chestertown and the surr</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -3058,7 +3074,7 @@
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>CE campus experience Q16 item 5 (QID21_5)</t>
+          <t>CE campus item QID21_8: SP23=Q16_8, SP24/25=Q16_9 (renumbered similarly)</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
@@ -3070,32 +3086,32 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>CE_campus_6</t>
+          <t>Know_WC_CE_mission</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>QID21_6</t>
+          <t>QID22</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>SP23:Q16_6 / SP24:Q16_6 / SP25:Q16_6</t>
+          <t>SP23:Q17 / SP24:Q17 / SP25:Q17</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - Washington College supports student civic engagement</t>
+          <t>Did you know that Washington College has civic engagement as a part of its mission?  “Washington College challenges and inspires emerging citizen leaders to discover lives of purpose and passion”?</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Likert-5</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>1=SD…5=SA</t>
+          <t>1=Yes, 0=No</t>
         </is>
       </c>
       <c r="G62" t="n">
@@ -3103,44 +3119,44 @@
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>CE campus experience Q16 item 6 (QID21_6)</t>
+          <t>Knew WC had CE in its mission?</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>[5, 1, 3, 2, 4]</t>
+          <t>[1, 0]</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>CE_campus_7</t>
+          <t>Agree_CE_mission</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>QID21_7</t>
+          <t>QID34</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>SP23:Q16_7 / SP24:Q16_8 / SP25:Q16_8</t>
+          <t>SP23:Q34 / SP24:Q34 / SP25:Q34</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - It is my responsibility to leave Washington College bette</t>
+          <t>Do you agree that civic engagement should be a part of our mission?</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Likert-5</t>
+          <t>binary</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>1=SD…5=SA</t>
+          <t>1=Yes, 0=No</t>
         </is>
       </c>
       <c r="G63" t="n">
@@ -3148,44 +3164,44 @@
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>CE campus item QID21_7: SP23=Q16_7, SP24/25=Q16_8 (renumbered due to new Q16_7 in SP24+)</t>
+          <t>Agrees CE should be in mission?</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>[5, 4, 3, 2, 1]</t>
+          <t>[1, 0]</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>CE_campus_8</t>
+          <t>WC_meeting_CE_mission</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>QID21_8</t>
+          <t>QID35</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>SP23:Q16_8 / SP24:Q16_9 / SP25:Q16_9</t>
+          <t>SP23:Q35 / SP24:Q35 / SP25:Q35</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>Please rate the extent to which you agree or disagree with the following questions about your experiences in/with the surrounding community. - It is my responsibility to leave Chestertown and the surr</t>
+          <t>Is Washington College meeting its civic engagement mission?</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Likert-5</t>
+          <t>categorical</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>1=SD…5=SA</t>
+          <t>1=No, 2=Somewhat, 3=Yes</t>
         </is>
       </c>
       <c r="G64" t="n">
@@ -3193,44 +3209,44 @@
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>CE campus item QID21_8: SP23=Q16_8, SP24/25=Q16_9 (renumbered similarly)</t>
+          <t>Is WC meeting CE mission?</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>[5, 4, 3, 2, 1]</t>
+          <t>[2, 0, 1]</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Know_WC_CE_mission</t>
+          <t>WC_CE_resources</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>QID22</t>
+          <t>QID36</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>SP23:Q17 / SP24:Q17 / SP25:Q17</t>
+          <t>SP23:Q36 / SP24:Q36 / SP25:Q36</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Did you know that Washington College has civic engagement as a part of its mission?  “Washington College challenges and inspires emerging citizen leaders to discover lives of purpose and passion”?</t>
+          <t>Does Washington College provide the required resources and opportunities for students to be civically engaged?</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>binary</t>
+          <t>categorical</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>1=Yes, 0=No</t>
+          <t>1=No, 2=Somewhat, 3=Yes</t>
         </is>
       </c>
       <c r="G65" t="n">
@@ -3238,44 +3254,44 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>Knew WC had CE in its mission?</t>
+          <t>Does WC provide CE resources?</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>[1, 0]</t>
+          <t>[2, 0, 1]</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Agree_CE_mission</t>
+          <t>Overall_CE_rating</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>QID34</t>
+          <t>QID23</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>SP23:Q34 / SP24:Q34 / SP25:Q34</t>
+          <t>SP23:Q18 / SP24:Q18 / SP25:Q18</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Do you agree that civic engagement should be a part of our mission?</t>
+          <t>How would you rate your overall civic engagement?</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>binary</t>
+          <t>Likert-5</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>1=Yes, 0=No</t>
+          <t>1=Not at all engaged…5=Extremely engaged</t>
         </is>
       </c>
       <c r="G66" t="n">
@@ -3283,44 +3299,36 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Agrees CE should be in mission?</t>
+          <t>Self-rated overall CE</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>[1, 0]</t>
+          <t>[1, 2, 3, 4, 5]</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>WC_meeting_CE_mission</t>
+          <t>CEdef_voting</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>QID35</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>SP23:Q35 / SP24:Q35 / SP25:Q35</t>
-        </is>
-      </c>
-      <c r="D67" t="inlineStr">
-        <is>
-          <t>Is Washington College meeting its civic engagement mission?</t>
-        </is>
-      </c>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
         <is>
-          <t>categorical</t>
+          <t>binary OHE</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>1=No, 2=Somewhat, 3=Yes</t>
+          <t>1=selected, 0=not selected, -9=missing</t>
         </is>
       </c>
       <c r="G67" t="n">
@@ -3328,44 +3336,36 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Is WC meeting CE mission?</t>
+          <t>CE definition: Voting</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>[2, 0, 1]</t>
+          <t>[1, 0]</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>WC_CE_resources</t>
+          <t>CEdef_volunteering</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>QID36</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>SP23:Q36 / SP24:Q36 / SP25:Q36</t>
-        </is>
-      </c>
-      <c r="D68" t="inlineStr">
-        <is>
-          <t>Does Washington College provide the required resources and opportunities for students to be civically engaged?</t>
-        </is>
-      </c>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
-          <t>categorical</t>
+          <t>binary OHE</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>1=No, 2=Somewhat, 3=Yes</t>
+          <t>1=selected, 0=not selected, -9=missing</t>
         </is>
       </c>
       <c r="G68" t="n">
@@ -3373,44 +3373,36 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Does WC provide CE resources?</t>
+          <t>CE definition: Volunteering or community service</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>[2, 0, 1]</t>
+          <t>[0, 1]</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Overall_CE_rating</t>
+          <t>CEdef_talking_community</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>QID23</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>SP23:Q18 / SP24:Q18 / SP25:Q18</t>
-        </is>
-      </c>
-      <c r="D69" t="inlineStr">
-        <is>
-          <t>How would you rate your overall civic engagement?</t>
-        </is>
-      </c>
+          <t>—</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Likert-5</t>
+          <t>binary OHE</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>1=Not at all engaged…5=Extremely engaged</t>
+          <t>1=selected, 0=not selected, -9=missing</t>
         </is>
       </c>
       <c r="G69" t="n">
@@ -3418,19 +3410,19 @@
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Self-rated overall CE</t>
+          <t>CE definition: Talking with people in the community</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>[1, 2, 3, 4, 5]</t>
+          <t>[0, 1]</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>CEdef_voting</t>
+          <t>CEdef_activism</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -3455,19 +3447,19 @@
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>CE definition: Voting</t>
+          <t>CE definition: Activism or awareness raising</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>[1, 0]</t>
+          <t>[0, 1]</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>CEdef_volunteering</t>
+          <t>CEdef_political</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -3492,7 +3484,7 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>CE definition: Volunteering or community service</t>
+          <t>CE definition: Political engagement</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
@@ -3504,7 +3496,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>CEdef_talking_community</t>
+          <t>CEdef_protesting</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -3529,7 +3521,7 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>CE definition: Talking with people in the community</t>
+          <t>CE definition: Protesting or rallying</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -3541,7 +3533,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>CEdef_activism</t>
+          <t>CEdef_teaching</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3566,7 +3558,7 @@
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>CE definition: Activism or awareness raising</t>
+          <t>CE definition: Teaching or mentorship</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
@@ -3578,7 +3570,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>CEdef_political</t>
+          <t>CEdef_fundraising</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -3603,7 +3595,7 @@
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>CE definition: Political engagement</t>
+          <t>CE definition: Fundraising</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
@@ -3615,7 +3607,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>CEdef_protesting</t>
+          <t>CEdef_arts_culture</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -3640,7 +3632,7 @@
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>CE definition: Protesting or rallying</t>
+          <t>CE definition: Attending community arts and culture events</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
@@ -3652,7 +3644,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>CEdef_teaching</t>
+          <t>CEdef_community_business</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -3677,7 +3669,7 @@
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>CE definition: Teaching or mentorship</t>
+          <t>CE definition: Contributing to community businesses with a social cause</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
@@ -3689,7 +3681,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>CEdef_fundraising</t>
+          <t>CEdef_donations</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -3714,7 +3706,7 @@
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>CE definition: Fundraising</t>
+          <t>CE definition: Making donations to charities</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
@@ -3726,7 +3718,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>CEdef_arts_culture</t>
+          <t>CEdef_research</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -3751,7 +3743,7 @@
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>CE definition: Attending community arts and culture events</t>
+          <t>CE definition: Participating in research with community members</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
@@ -3763,7 +3755,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>CEdef_community_business</t>
+          <t>CEdef_service_learning</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -3788,7 +3780,7 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>CE definition: Contributing to community businesses with a social cause</t>
+          <t>CE definition: Service-learning experiences with a class</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -3800,7 +3792,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>CEdef_donations</t>
+          <t>Media_repost_events</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -3825,7 +3817,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>CE definition: Making donations to charities</t>
+          <t>Media CE: Reposting information about current events</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -3837,7 +3829,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>CEdef_research</t>
+          <t>Media_sign_petition</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -3862,7 +3854,7 @@
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>CE definition: Participating in research with community members</t>
+          <t>Media CE: Signing online petitions</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
@@ -3874,7 +3866,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>CEdef_service_learning</t>
+          <t>Media_follow_news</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -3899,19 +3891,19 @@
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>CE definition: Service-learning experiences with a class</t>
+          <t>Media CE: Following accounts/pages about current events</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>[0, 1]</t>
+          <t>[1, 0]</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Media_repost_events</t>
+          <t>Media_follow_officials</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -3936,7 +3928,7 @@
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Media CE: Reposting information about current events</t>
+          <t>Media CE: Following elected officials on social media</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
@@ -3948,7 +3940,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Media_sign_petition</t>
+          <t>Media_debate_opinions</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -3973,7 +3965,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Media CE: Signing online petitions</t>
+          <t>Media CE: Debating opinions with others who disagree</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -3985,7 +3977,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Media_follow_news</t>
+          <t>Media_like_posts</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -4010,19 +4002,19 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Media CE: Following accounts/pages about current events</t>
+          <t>Media CE: Liking posts about current events</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>[1, 0]</t>
+          <t>[0, 1]</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Media_follow_officials</t>
+          <t>Media_post_opinions</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -4047,7 +4039,7 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>Media CE: Following elected officials on social media</t>
+          <t>Media CE: Posting own opinions about current events</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
@@ -4059,7 +4051,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Media_debate_opinions</t>
+          <t>News_The_Elm</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -4084,19 +4076,19 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>Media CE: Debating opinions with others who disagree</t>
+          <t>Local news: The Elm</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>[0, 1]</t>
+          <t>[1, 0]</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Media_like_posts</t>
+          <t>News_Kent_County</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -4121,7 +4113,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Media CE: Liking posts about current events</t>
+          <t>Local news: Kent County News</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
@@ -4133,7 +4125,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Media_post_opinions</t>
+          <t>News_Chestertown_Spy</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -4158,7 +4150,7 @@
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>Media CE: Posting own opinions about current events</t>
+          <t>Local news: The Chestertown Spy</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
@@ -4170,7 +4162,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>News_The_Elm</t>
+          <t>News_Eastern_Shore_Post</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -4195,19 +4187,19 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Local news: The Elm</t>
+          <t>Local news: Eastern Shore Post</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>[1, 0]</t>
+          <t>[0, 1]</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>News_Kent_County</t>
+          <t>News_Shore_Daily</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -4232,7 +4224,7 @@
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>Local news: Kent County News</t>
+          <t>Local news: Shore Daily News</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
@@ -4244,7 +4236,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>News_Chestertown_Spy</t>
+          <t>News_Delmarva_Now</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -4269,121 +4261,10 @@
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>Local news: The Chestertown Spy</t>
+          <t>Local news: Delmarva Now</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
-        <is>
-          <t>[0, 1]</t>
-        </is>
-      </c>
-    </row>
-    <row r="93">
-      <c r="A93" t="inlineStr">
-        <is>
-          <t>News_Eastern_Shore_Post</t>
-        </is>
-      </c>
-      <c r="B93" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C93" t="inlineStr"/>
-      <c r="D93" t="inlineStr"/>
-      <c r="E93" t="inlineStr">
-        <is>
-          <t>binary OHE</t>
-        </is>
-      </c>
-      <c r="F93" t="inlineStr">
-        <is>
-          <t>1=selected, 0=not selected, -9=missing</t>
-        </is>
-      </c>
-      <c r="G93" t="n">
-        <v>-9</v>
-      </c>
-      <c r="H93" t="inlineStr">
-        <is>
-          <t>Local news: Eastern Shore Post</t>
-        </is>
-      </c>
-      <c r="I93" t="inlineStr">
-        <is>
-          <t>[0, 1]</t>
-        </is>
-      </c>
-    </row>
-    <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>News_Shore_Daily</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
-      <c r="E94" t="inlineStr">
-        <is>
-          <t>binary OHE</t>
-        </is>
-      </c>
-      <c r="F94" t="inlineStr">
-        <is>
-          <t>1=selected, 0=not selected, -9=missing</t>
-        </is>
-      </c>
-      <c r="G94" t="n">
-        <v>-9</v>
-      </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>Local news: Shore Daily News</t>
-        </is>
-      </c>
-      <c r="I94" t="inlineStr">
-        <is>
-          <t>[0, 1]</t>
-        </is>
-      </c>
-    </row>
-    <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>News_Delmarva_Now</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr">
-        <is>
-          <t>—</t>
-        </is>
-      </c>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
-      <c r="E95" t="inlineStr">
-        <is>
-          <t>binary OHE</t>
-        </is>
-      </c>
-      <c r="F95" t="inlineStr">
-        <is>
-          <t>1=selected, 0=not selected, -9=missing</t>
-        </is>
-      </c>
-      <c r="G95" t="n">
-        <v>-9</v>
-      </c>
-      <c r="H95" t="inlineStr">
-        <is>
-          <t>Local news: Delmarva Now</t>
-        </is>
-      </c>
-      <c r="I95" t="inlineStr">
         <is>
           <t>[0, 1]</t>
         </is>

</xml_diff>